<commit_message>
opdateret tidsplan med programmerings del startingopdateret tidsplan med programmerings delopdateret tidsplan med programmerings del
</commit_message>
<xml_diff>
--- a/Tidsplan_Vinkaelder.xlsx
+++ b/Tidsplan_Vinkaelder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Project\VinkaelderProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACAD64DF-1E5A-4F4A-B2CD-B1B748B9CD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4189DDD-16E1-4520-B6A8-D0FC9EC67A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{03DAF2AD-776B-4C12-BC18-C19A447D28B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Datoer/Opgaver</t>
   </si>
@@ -71,17 +71,36 @@
     <t>Dokumentation af arbejde</t>
   </si>
   <si>
-    <t>Programmering</t>
+    <t xml:space="preserve">Program brugerfladedesign </t>
+  </si>
+  <si>
+    <t>Brugerflade, minimum</t>
+  </si>
+  <si>
+    <t>Brugerflade, selvvalgte ure</t>
+  </si>
+  <si>
+    <t>Backend, værdiproduktion</t>
+  </si>
+  <si>
+    <t>Newsfeed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,13 +144,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,11 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DA85DF-4947-4396-AFAF-3FDC5AEDCB1D}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J20" sqref="J20"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,11 +486,15 @@
     <col min="9" max="9" width="28.5703125" customWidth="1"/>
     <col min="10" max="10" width="26.85546875" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="15" width="42.28515625" customWidth="1"/>
+    <col min="12" max="12" width="32.140625" customWidth="1"/>
+    <col min="13" max="13" width="28.5703125" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" customWidth="1"/>
+    <col min="15" max="15" width="26" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,23 +531,36 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44910</v>
       </c>
       <c r="B2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44911</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44914</v>
       </c>
@@ -534,8 +571,10 @@
       <c r="G4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44915</v>
       </c>
@@ -544,9 +583,13 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44928</v>
       </c>
@@ -554,46 +597,64 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44929</v>
       </c>
       <c r="E7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="5"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44930</v>
       </c>
       <c r="E8" s="3"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="5"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44931</v>
       </c>
       <c r="E9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="5"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44932</v>
       </c>
       <c r="E10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tilføjet manglene felt i tidsplan omkring router/switch
</commit_message>
<xml_diff>
--- a/Tidsplan_Vinkaelder.xlsx
+++ b/Tidsplan_Vinkaelder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Project\VinkaelderProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4189DDD-16E1-4520-B6A8-D0FC9EC67A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200933DA-E37B-41A7-A8FD-D45F1CCF3044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{03DAF2AD-776B-4C12-BC18-C19A447D28B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Datoer/Opgaver</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Newsfeed</t>
+  </si>
+  <si>
+    <t>Konfiguration af router/switch</t>
   </si>
 </sst>
 </file>
@@ -144,13 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -466,11 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DA85DF-4947-4396-AFAF-3FDC5AEDCB1D}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,10 +493,10 @@
     <col min="14" max="14" width="26.85546875" customWidth="1"/>
     <col min="15" max="15" width="26" customWidth="1"/>
     <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" customWidth="1"/>
+    <col min="17" max="17" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,24 +545,27 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44910</v>
       </c>
       <c r="B2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44911</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44914</v>
       </c>
@@ -572,9 +577,9 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44915</v>
       </c>
@@ -588,8 +593,9 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44928</v>
       </c>
@@ -597,11 +603,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="5"/>
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44929</v>
       </c>
@@ -609,52 +615,49 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="5"/>
       <c r="M7" s="2"/>
       <c r="N7" s="3"/>
       <c r="O7" s="2"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44930</v>
       </c>
       <c r="E8" s="3"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="5"/>
       <c r="M8" s="2"/>
       <c r="N8" s="3"/>
       <c r="O8" s="2"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44931</v>
       </c>
       <c r="E9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="5"/>
       <c r="M9" s="4"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44932</v>
       </c>
       <c r="E10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="5"/>
       <c r="M10" s="4"/>
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opdateret tidsplan efter de højre magters ideal
</commit_message>
<xml_diff>
--- a/Tidsplan_Vinkaelder.xlsx
+++ b/Tidsplan_Vinkaelder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Project\VinkaelderProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200933DA-E37B-41A7-A8FD-D45F1CCF3044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8EFEDD-C4FF-438B-B793-EF6F22164968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{03DAF2AD-776B-4C12-BC18-C19A447D28B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Datoer/Opgaver</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Installation af klienter</t>
   </si>
   <si>
-    <t>Opsætning af printere</t>
-  </si>
-  <si>
     <t>Serverkonfiguration (DHCP)</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>Konfiguration af router/switch</t>
+  </si>
+  <si>
+    <t>Rapportskrivning</t>
+  </si>
+  <si>
+    <t>Retskrivning</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +137,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -147,13 +156,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,11 +478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DA85DF-4947-4396-AFAF-3FDC5AEDCB1D}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,22 +491,24 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
     <col min="10" max="10" width="26.85546875" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="32.140625" customWidth="1"/>
-    <col min="13" max="13" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
     <col min="14" max="14" width="26.85546875" customWidth="1"/>
-    <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="28" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,38 +560,40 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44910</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44911</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44914</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44915</v>
       </c>
@@ -587,77 +601,77 @@
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44928</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="5"/>
-      <c r="O6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="L6" s="5"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44929</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="6"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44930</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="6"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44931</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="6"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44932</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="K10" s="2"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="6"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>

</xml_diff>